<commit_message>
Update Column/View Shipping App
</commit_message>
<xml_diff>
--- a/Microservices/FilesMicroservice/Files.Api/wwwroot/templates/ShippingPlanTemplate.xlsx
+++ b/Microservices/FilesMicroservice/Files.Api/wwwroot/templates/ShippingPlanTemplate.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ShippingPlanId</t>
   </si>
@@ -45,6 +45,24 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>BillTo</t>
+  </si>
+  <si>
+    <t>BillToAddress</t>
+  </si>
+  <si>
+    <t>ShipTo</t>
+  </si>
+  <si>
+    <t>ShipToAddress</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>ProductLine</t>
   </si>
 </sst>
 </file>
@@ -114,7 +132,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -131,6 +149,12 @@
     <col min="9" max="9" width="30" customWidth="1" style="1"/>
     <col min="10" max="10" width="30" customWidth="1" style="1"/>
     <col min="11" max="11" width="30" customWidth="1" style="1"/>
+    <col min="12" max="12" width="30" customWidth="1" style="1"/>
+    <col min="13" max="13" width="30" customWidth="1" style="1"/>
+    <col min="14" max="14" width="30" customWidth="1" style="1"/>
+    <col min="15" max="15" width="30" customWidth="1" style="1"/>
+    <col min="16" max="16" width="30" customWidth="1" style="1"/>
+    <col min="17" max="17" width="30" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -167,6 +191,24 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <headerFooter/>

</xml_diff>

<commit_message>
Update Import - Add Barcode - Update ShippingPlan/WorkOrder/Movement...
</commit_message>
<xml_diff>
--- a/Microservices/FilesMicroservice/Files.Api/wwwroot/templates/ShippingPlanTemplate.xlsx
+++ b/Microservices/FilesMicroservice/Files.Api/wwwroot/templates/ShippingPlanTemplate.xlsx
@@ -20,10 +20,10 @@
     <t>PurchaseOrder</t>
   </si>
   <si>
-    <t>SalesID</t>
-  </si>
-  <si>
-    <t>SemlineNumber</t>
+    <t>SalesOrder</t>
+  </si>
+  <si>
+    <t>SalelineNumber</t>
   </si>
   <si>
     <t>ProductNumber</t>

</xml_diff>